<commit_message>
Feat: Mudança da cor
</commit_message>
<xml_diff>
--- a/Resumo_Equipe_2025-07-14.xlsx
+++ b/Resumo_Equipe_2025-07-14.xlsx
@@ -499,7 +499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,14 +607,14 @@
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>trste</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
@@ -624,11 +624,11 @@
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="D13" s="8" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E13" s="9">
         <f>IFERROR(VLOOKUP(B13,TabelaPrecos,2,FALSE)*D13,"-")</f>
@@ -648,11 +648,11 @@
       </c>
       <c r="C14" s="7" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="D14" s="8" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E14" s="9">
         <f>IFERROR(VLOOKUP(B14,TabelaPrecos,2,FALSE)*D14,"-")</f>
@@ -672,11 +672,11 @@
       </c>
       <c r="C15" s="7" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="D15" s="8" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E15" s="9">
         <f>IFERROR(VLOOKUP(B15,TabelaPrecos,2,FALSE)*D15,"-")</f>
@@ -696,11 +696,11 @@
       </c>
       <c r="C16" s="7" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="D16" s="8" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E16" s="9">
         <f>IFERROR(VLOOKUP(B16,TabelaPrecos,2,FALSE)*D16,"-")</f>
@@ -720,11 +720,11 @@
       </c>
       <c r="C17" s="7" t="inlineStr">
         <is>
-          <t>Acompanhamento de Sondagens</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="D17" s="8" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="E17" s="9">
         <f>IFERROR(VLOOKUP(B17,TabelaPrecos,2,FALSE)*D17,"-")</f>
@@ -813,12 +813,12 @@
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C22" s="7" t="inlineStr">
@@ -835,57 +835,74 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="inlineStr">
-        <is>
-          <t>Drenagem</t>
-        </is>
+      <c r="A23" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C23" s="7" t="inlineStr">
+        <is>
+          <t>Coordenação</t>
+        </is>
+      </c>
+      <c r="D23" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <f>IFERROR(VLOOKUP(B23,TabelaPrecos,2,FALSE)*D23,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="inlineStr">
-        <is>
-          <t>teste1</t>
-        </is>
-      </c>
-      <c r="B24" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C24" s="7" t="inlineStr">
-        <is>
-          <t>Drenagem</t>
-        </is>
-      </c>
-      <c r="D24" s="8" t="n">
-        <v>160</v>
-      </c>
-      <c r="E24" s="9">
-        <f>IFERROR(VLOOKUP(B24,TabelaPrecos,2,FALSE)*D24,"-")</f>
-        <v/>
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Desapropriação</t>
+        </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="6" t="inlineStr">
-        <is>
-          <t>Estruturas</t>
-        </is>
+      <c r="A25" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="B25" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C25" s="7" t="inlineStr">
+        <is>
+          <t>Desapropriação</t>
+        </is>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <f>IFERROR(VLOOKUP(B25,TabelaPrecos,2,FALSE)*D25,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B26" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C26" s="7" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Desapropriação</t>
         </is>
       </c>
       <c r="D26" s="8" t="n">
@@ -899,17 +916,17 @@
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B27" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C27" s="7" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Desapropriação</t>
         </is>
       </c>
       <c r="D27" s="8" t="n">
@@ -923,17 +940,17 @@
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B28" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C28" s="7" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Desapropriação</t>
         </is>
       </c>
       <c r="D28" s="8" t="n">
@@ -957,7 +974,7 @@
       </c>
       <c r="C29" s="7" t="inlineStr">
         <is>
-          <t>Estruturas</t>
+          <t>Desapropriação</t>
         </is>
       </c>
       <c r="D29" s="8" t="n">
@@ -971,7 +988,7 @@
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>Estudo de Alternativa</t>
+          <t>Drenagem</t>
         </is>
       </c>
     </row>
@@ -988,7 +1005,7 @@
       </c>
       <c r="C31" s="7" t="inlineStr">
         <is>
-          <t>Estudo de Alternativa</t>
+          <t>Drenagem</t>
         </is>
       </c>
       <c r="D31" s="8" t="n">
@@ -1002,17 +1019,17 @@
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B32" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C32" s="7" t="inlineStr">
         <is>
-          <t>Estudo de Alternativa</t>
+          <t>Drenagem</t>
         </is>
       </c>
       <c r="D32" s="8" t="n">
@@ -1026,17 +1043,17 @@
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B33" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C33" s="7" t="inlineStr">
         <is>
-          <t>Estudo de Alternativa</t>
+          <t>Drenagem</t>
         </is>
       </c>
       <c r="D33" s="8" t="n">
@@ -1048,26 +1065,43 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="inlineStr">
-        <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
-        </is>
+      <c r="A34" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="B34" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>Drenagem</t>
+        </is>
+      </c>
+      <c r="D34" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="9">
+        <f>IFERROR(VLOOKUP(B34,TabelaPrecos,2,FALSE)*D34,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="inlineStr">
         <is>
-          <t>teste23</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B35" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C35" s="7" t="inlineStr">
         <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
+          <t>Drenagem</t>
         </is>
       </c>
       <c r="D35" s="8" t="n">
@@ -1079,43 +1113,26 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Sênior</t>
-        </is>
-      </c>
-      <c r="B36" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Sênior</t>
-        </is>
-      </c>
-      <c r="C36" s="7" t="inlineStr">
-        <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
-        </is>
-      </c>
-      <c r="D36" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="9">
-        <f>IFERROR(VLOOKUP(B36,TabelaPrecos,2,FALSE)*D36,"-")</f>
-        <v/>
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>Estruturas</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B37" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C37" s="7" t="inlineStr">
         <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
+          <t>Estruturas</t>
         </is>
       </c>
       <c r="D37" s="8" t="n">
@@ -1129,17 +1146,17 @@
     <row r="38">
       <c r="A38" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B38" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C38" s="7" t="inlineStr">
         <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
+          <t>Estruturas</t>
         </is>
       </c>
       <c r="D38" s="8" t="n">
@@ -1151,30 +1168,47 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="inlineStr">
-        <is>
-          <t>Estudos Hidrológicos</t>
-        </is>
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="B39" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C39" s="7" t="inlineStr">
+        <is>
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="D39" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="9">
+        <f>IFERROR(VLOOKUP(B39,TabelaPrecos,2,FALSE)*D39,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="7" t="inlineStr">
         <is>
-          <t>teste1</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B40" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C40" s="7" t="inlineStr">
         <is>
-          <t>Estudos Hidrológicos</t>
+          <t>Estruturas</t>
         </is>
       </c>
       <c r="D40" s="8" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="E40" s="9">
         <f>IFERROR(VLOOKUP(B40,TabelaPrecos,2,FALSE)*D40,"-")</f>
@@ -1182,50 +1216,50 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="inlineStr">
-        <is>
-          <t>Geologia</t>
-        </is>
+      <c r="A41" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B41" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C41" s="7" t="inlineStr">
+        <is>
+          <t>Estruturas</t>
+        </is>
+      </c>
+      <c r="D41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="9">
+        <f>IFERROR(VLOOKUP(B41,TabelaPrecos,2,FALSE)*D41,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B42" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C42" s="7" t="inlineStr">
-        <is>
-          <t>Geologia</t>
-        </is>
-      </c>
-      <c r="D42" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="9">
-        <f>IFERROR(VLOOKUP(B42,TabelaPrecos,2,FALSE)*D42,"-")</f>
-        <v/>
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>Estudo de Alternativa</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="7" t="inlineStr">
         <is>
-          <t>teste23</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B43" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C43" s="7" t="inlineStr">
         <is>
-          <t>Geologia</t>
+          <t>Estudo de Alternativa</t>
         </is>
       </c>
       <c r="D43" s="8" t="n">
@@ -1239,17 +1273,17 @@
     <row r="44">
       <c r="A44" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B44" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C44" s="7" t="inlineStr">
         <is>
-          <t>Geologia</t>
+          <t>Estudo de Alternativa</t>
         </is>
       </c>
       <c r="D44" s="8" t="n">
@@ -1263,17 +1297,17 @@
     <row r="45">
       <c r="A45" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B45" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C45" s="7" t="inlineStr">
         <is>
-          <t>Geologia</t>
+          <t>Estudo de Alternativa</t>
         </is>
       </c>
       <c r="D45" s="8" t="n">
@@ -1285,50 +1319,50 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="inlineStr">
-        <is>
-          <t>Geometria</t>
-        </is>
+      <c r="A46" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B46" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>Estudo de Alternativa</t>
+        </is>
+      </c>
+      <c r="D46" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="9">
+        <f>IFERROR(VLOOKUP(B46,TabelaPrecos,2,FALSE)*D46,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B47" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C47" s="7" t="inlineStr">
-        <is>
-          <t>Geometria</t>
-        </is>
-      </c>
-      <c r="D47" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="9">
-        <f>IFERROR(VLOOKUP(B47,TabelaPrecos,2,FALSE)*D47,"-")</f>
-        <v/>
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>Estudos Geológicos-Geotécnicos</t>
+        </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B48" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C48" s="7" t="inlineStr">
         <is>
-          <t>Geometria</t>
+          <t>Estudos Geológicos-Geotécnicos</t>
         </is>
       </c>
       <c r="D48" s="8" t="n">
@@ -1342,17 +1376,17 @@
     <row r="49">
       <c r="A49" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B49" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C49" s="7" t="inlineStr">
         <is>
-          <t>Geometria</t>
+          <t>Estudos Geológicos-Geotécnicos</t>
         </is>
       </c>
       <c r="D49" s="8" t="n">
@@ -1366,17 +1400,17 @@
     <row r="50">
       <c r="A50" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B50" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C50" s="7" t="inlineStr">
         <is>
-          <t>Geometria</t>
+          <t>Estudos Geológicos-Geotécnicos</t>
         </is>
       </c>
       <c r="D50" s="8" t="n">
@@ -1390,17 +1424,17 @@
     <row r="51">
       <c r="A51" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B51" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C51" s="7" t="inlineStr">
         <is>
-          <t>Geometria</t>
+          <t>Estudos Geológicos-Geotécnicos</t>
         </is>
       </c>
       <c r="D51" s="8" t="n">
@@ -1412,50 +1446,50 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="6" t="inlineStr">
-        <is>
-          <t>Geotecnia</t>
-        </is>
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B52" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>Estudos Geológicos-Geotécnicos</t>
+        </is>
+      </c>
+      <c r="D52" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="9">
+        <f>IFERROR(VLOOKUP(B52,TabelaPrecos,2,FALSE)*D52,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B53" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C53" s="7" t="inlineStr">
-        <is>
-          <t>Geotecnia</t>
-        </is>
-      </c>
-      <c r="D53" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="9">
-        <f>IFERROR(VLOOKUP(B53,TabelaPrecos,2,FALSE)*D53,"-")</f>
-        <v/>
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Estudos Hidrológicos</t>
+        </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B54" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C54" s="7" t="inlineStr">
         <is>
-          <t>Geotecnia</t>
+          <t>Estudos Hidrológicos</t>
         </is>
       </c>
       <c r="D54" s="8" t="n">
@@ -1469,17 +1503,17 @@
     <row r="55">
       <c r="A55" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B55" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C55" s="7" t="inlineStr">
         <is>
-          <t>Geotecnia</t>
+          <t>Estudos Hidrológicos</t>
         </is>
       </c>
       <c r="D55" s="8" t="n">
@@ -1493,17 +1527,17 @@
     <row r="56">
       <c r="A56" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B56" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C56" s="7" t="inlineStr">
         <is>
-          <t>Geotecnia</t>
+          <t>Estudos Hidrológicos</t>
         </is>
       </c>
       <c r="D56" s="8" t="n">
@@ -1517,17 +1551,17 @@
     <row r="57">
       <c r="A57" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B57" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C57" s="7" t="inlineStr">
         <is>
-          <t>Geotecnia</t>
+          <t>Estudos Hidrológicos</t>
         </is>
       </c>
       <c r="D57" s="8" t="n">
@@ -1539,50 +1573,50 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="6" t="inlineStr">
-        <is>
-          <t>Pavimento</t>
-        </is>
+      <c r="A58" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B58" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>Estudos Hidrológicos</t>
+        </is>
+      </c>
+      <c r="D58" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="9">
+        <f>IFERROR(VLOOKUP(B58,TabelaPrecos,2,FALSE)*D58,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B59" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C59" s="7" t="inlineStr">
-        <is>
-          <t>Pavimento</t>
-        </is>
-      </c>
-      <c r="D59" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="9">
-        <f>IFERROR(VLOOKUP(B59,TabelaPrecos,2,FALSE)*D59,"-")</f>
-        <v/>
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>Geologia</t>
+        </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B60" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C60" s="7" t="inlineStr">
         <is>
-          <t>Pavimento</t>
+          <t>Geologia</t>
         </is>
       </c>
       <c r="D60" s="8" t="n">
@@ -1596,17 +1630,17 @@
     <row r="61">
       <c r="A61" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B61" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C61" s="7" t="inlineStr">
         <is>
-          <t>Pavimento</t>
+          <t>Geologia</t>
         </is>
       </c>
       <c r="D61" s="8" t="n">
@@ -1618,26 +1652,43 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Desapropriação</t>
-        </is>
+      <c r="A62" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>Geologia</t>
+        </is>
+      </c>
+      <c r="D62" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="9">
+        <f>IFERROR(VLOOKUP(B62,TabelaPrecos,2,FALSE)*D62,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B63" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C63" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Desapropriação</t>
+          <t>Geologia</t>
         </is>
       </c>
       <c r="D63" s="8" t="n">
@@ -1651,17 +1702,17 @@
     <row r="64">
       <c r="A64" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B64" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C64" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Desapropriação</t>
+          <t>Geologia</t>
         </is>
       </c>
       <c r="D64" s="8" t="n">
@@ -1673,43 +1724,26 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Pleno</t>
-        </is>
-      </c>
-      <c r="B65" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Pleno</t>
-        </is>
-      </c>
-      <c r="C65" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Desapropriação</t>
-        </is>
-      </c>
-      <c r="D65" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" s="9">
-        <f>IFERROR(VLOOKUP(B65,TabelaPrecos,2,FALSE)*D65,"-")</f>
-        <v/>
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>Geometria</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B66" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C66" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Desapropriação</t>
+          <t>Geometria</t>
         </is>
       </c>
       <c r="D66" s="8" t="n">
@@ -1723,17 +1757,17 @@
     <row r="67">
       <c r="A67" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B67" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C67" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Desapropriação</t>
+          <t>Geometria</t>
         </is>
       </c>
       <c r="D67" s="8" t="n">
@@ -1745,26 +1779,43 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Interferência</t>
-        </is>
+      <c r="A68" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="B68" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>Geometria</t>
+        </is>
+      </c>
+      <c r="D68" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="9">
+        <f>IFERROR(VLOOKUP(B68,TabelaPrecos,2,FALSE)*D68,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B69" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C69" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Interferência</t>
+          <t>Geometria</t>
         </is>
       </c>
       <c r="D69" s="8" t="n">
@@ -1778,17 +1829,17 @@
     <row r="70">
       <c r="A70" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B70" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C70" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Interferência</t>
+          <t>Geometria</t>
         </is>
       </c>
       <c r="D70" s="8" t="n">
@@ -1800,43 +1851,26 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Pleno</t>
-        </is>
-      </c>
-      <c r="B71" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Pleno</t>
-        </is>
-      </c>
-      <c r="C71" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Interferência</t>
-        </is>
-      </c>
-      <c r="D71" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E71" s="9">
-        <f>IFERROR(VLOOKUP(B71,TabelaPrecos,2,FALSE)*D71,"-")</f>
-        <v/>
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>Geotecnia</t>
+        </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B72" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C72" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Interferência</t>
+          <t>Geotecnia</t>
         </is>
       </c>
       <c r="D72" s="8" t="n">
@@ -1850,17 +1884,17 @@
     <row r="73">
       <c r="A73" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B73" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C73" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Interferência</t>
+          <t>Geotecnia</t>
         </is>
       </c>
       <c r="D73" s="8" t="n">
@@ -1872,26 +1906,43 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Obras Complementares</t>
-        </is>
+      <c r="A74" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="B74" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>Geotecnia</t>
+        </is>
+      </c>
+      <c r="D74" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="9">
+        <f>IFERROR(VLOOKUP(B74,TabelaPrecos,2,FALSE)*D74,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B75" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C75" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Obras Complementares</t>
+          <t>Geotecnia</t>
         </is>
       </c>
       <c r="D75" s="8" t="n">
@@ -1903,43 +1954,26 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Júnior</t>
-        </is>
-      </c>
-      <c r="B76" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Júnior</t>
-        </is>
-      </c>
-      <c r="C76" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Obras Complementares</t>
-        </is>
-      </c>
-      <c r="D76" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" s="9">
-        <f>IFERROR(VLOOKUP(B76,TabelaPrecos,2,FALSE)*D76,"-")</f>
-        <v/>
+      <c r="A76" s="6" t="inlineStr">
+        <is>
+          <t>Interferência</t>
+        </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B77" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C77" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Obras Complementares</t>
+          <t>Interferência</t>
         </is>
       </c>
       <c r="D77" s="8" t="n">
@@ -1951,26 +1985,43 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Paisagismo</t>
-        </is>
+      <c r="A78" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="B78" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>Interferência</t>
+        </is>
+      </c>
+      <c r="D78" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="9">
+        <f>IFERROR(VLOOKUP(B78,TabelaPrecos,2,FALSE)*D78,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B79" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C79" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Paisagismo</t>
+          <t>Interferência</t>
         </is>
       </c>
       <c r="D79" s="8" t="n">
@@ -1984,17 +2035,17 @@
     <row r="80">
       <c r="A80" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B80" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C80" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Paisagismo</t>
+          <t>Interferência</t>
         </is>
       </c>
       <c r="D80" s="8" t="n">
@@ -2008,17 +2059,17 @@
     <row r="81">
       <c r="A81" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B81" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C81" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Paisagismo</t>
+          <t>Interferência</t>
         </is>
       </c>
       <c r="D81" s="8" t="n">
@@ -2030,43 +2081,26 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Júnior</t>
-        </is>
-      </c>
-      <c r="B82" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Júnior</t>
-        </is>
-      </c>
-      <c r="C82" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Paisagismo</t>
-        </is>
-      </c>
-      <c r="D82" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E82" s="9">
-        <f>IFERROR(VLOOKUP(B82,TabelaPrecos,2,FALSE)*D82,"-")</f>
-        <v/>
+      <c r="A82" s="6" t="inlineStr">
+        <is>
+          <t>Obras Complementares</t>
+        </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B83" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C83" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Paisagismo</t>
+          <t>Obras Complementares</t>
         </is>
       </c>
       <c r="D83" s="8" t="n">
@@ -2078,26 +2112,43 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Parada de Ônibus</t>
-        </is>
+      <c r="A84" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="B84" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>Obras Complementares</t>
+        </is>
+      </c>
+      <c r="D84" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="9">
+        <f>IFERROR(VLOOKUP(B84,TabelaPrecos,2,FALSE)*D84,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B85" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C85" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Parada de Ônibus</t>
+          <t>Obras Complementares</t>
         </is>
       </c>
       <c r="D85" s="8" t="n">
@@ -2109,43 +2160,26 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Sênior</t>
-        </is>
-      </c>
-      <c r="B86" s="7" t="inlineStr">
-        <is>
-          <t>Eng. Sênior</t>
-        </is>
-      </c>
-      <c r="C86" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Parada de Ônibus</t>
-        </is>
-      </c>
-      <c r="D86" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E86" s="9">
-        <f>IFERROR(VLOOKUP(B86,TabelaPrecos,2,FALSE)*D86,"-")</f>
-        <v/>
+      <c r="A86" s="6" t="inlineStr">
+        <is>
+          <t>Paisagismo</t>
+        </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B87" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C87" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Parada de Ônibus</t>
+          <t>Paisagismo</t>
         </is>
       </c>
       <c r="D87" s="8" t="n">
@@ -2159,17 +2193,17 @@
     <row r="88">
       <c r="A88" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B88" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C88" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Parada de Ônibus</t>
+          <t>Paisagismo</t>
         </is>
       </c>
       <c r="D88" s="8" t="n">
@@ -2183,17 +2217,17 @@
     <row r="89">
       <c r="A89" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B89" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C89" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Parada de Ônibus</t>
+          <t>Paisagismo</t>
         </is>
       </c>
       <c r="D89" s="8" t="n">
@@ -2205,50 +2239,50 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
-        </is>
+      <c r="A90" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B90" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>Paisagismo</t>
+        </is>
+      </c>
+      <c r="D90" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="9">
+        <f>IFERROR(VLOOKUP(B90,TabelaPrecos,2,FALSE)*D90,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B91" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C91" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
-        </is>
-      </c>
-      <c r="D91" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" s="9">
-        <f>IFERROR(VLOOKUP(B91,TabelaPrecos,2,FALSE)*D91,"-")</f>
-        <v/>
+      <c r="A91" s="6" t="inlineStr">
+        <is>
+          <t>Parada de Ônibus</t>
+        </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B92" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C92" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
+          <t>Parada de Ônibus</t>
         </is>
       </c>
       <c r="D92" s="8" t="n">
@@ -2262,17 +2296,17 @@
     <row r="93">
       <c r="A93" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B93" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C93" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
+          <t>Parada de Ônibus</t>
         </is>
       </c>
       <c r="D93" s="8" t="n">
@@ -2286,17 +2320,17 @@
     <row r="94">
       <c r="A94" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B94" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C94" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
+          <t>Parada de Ônibus</t>
         </is>
       </c>
       <c r="D94" s="8" t="n">
@@ -2310,17 +2344,17 @@
     <row r="95">
       <c r="A95" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B95" s="7" t="inlineStr">
         <is>
-          <t>Coordenador</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C95" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
+          <t>Parada de Ônibus</t>
         </is>
       </c>
       <c r="D95" s="8" t="n">
@@ -2332,34 +2366,34 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="6" t="inlineStr">
-        <is>
-          <t>Projeto de Topografia</t>
-        </is>
+      <c r="A96" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B96" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>Parada de Ônibus</t>
+        </is>
+      </c>
+      <c r="D96" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" s="9">
+        <f>IFERROR(VLOOKUP(B96,TabelaPrecos,2,FALSE)*D96,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B97" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C97" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Topografia</t>
-        </is>
-      </c>
-      <c r="D97" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E97" s="9">
-        <f>IFERROR(VLOOKUP(B97,TabelaPrecos,2,FALSE)*D97,"-")</f>
-        <v/>
+      <c r="A97" s="6" t="inlineStr">
+        <is>
+          <t>Passarelas e de Pedestres</t>
+        </is>
       </c>
     </row>
     <row r="98">
@@ -2375,7 +2409,7 @@
       </c>
       <c r="C98" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Topografia</t>
+          <t>Passarelas e de Pedestres</t>
         </is>
       </c>
       <c r="D98" s="8" t="n">
@@ -2389,17 +2423,17 @@
     <row r="99">
       <c r="A99" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B99" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C99" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Topografia</t>
+          <t>Passarelas e de Pedestres</t>
         </is>
       </c>
       <c r="D99" s="8" t="n">
@@ -2413,17 +2447,17 @@
     <row r="100">
       <c r="A100" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B100" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C100" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Topografia</t>
+          <t>Passarelas e de Pedestres</t>
         </is>
       </c>
       <c r="D100" s="8" t="n">
@@ -2435,50 +2469,50 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="7" t="inlineStr">
-        <is>
-          <t>Coordenador</t>
-        </is>
-      </c>
-      <c r="B101" s="7" t="inlineStr">
-        <is>
-          <t>Coordenador</t>
-        </is>
-      </c>
-      <c r="C101" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Topografia</t>
-        </is>
-      </c>
-      <c r="D101" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E101" s="9">
-        <f>IFERROR(VLOOKUP(B101,TabelaPrecos,2,FALSE)*D101,"-")</f>
-        <v/>
+      <c r="A101" s="6" t="inlineStr">
+        <is>
+          <t>Pavimento</t>
+        </is>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="6" t="inlineStr">
-        <is>
-          <t>Sinalização</t>
-        </is>
+      <c r="A102" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="B102" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C102" s="7" t="inlineStr">
+        <is>
+          <t>Pavimento</t>
+        </is>
+      </c>
+      <c r="D102" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="9">
+        <f>IFERROR(VLOOKUP(B102,TabelaPrecos,2,FALSE)*D102,"-")</f>
+        <v/>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="B103" s="7" t="inlineStr">
         <is>
-          <t>Estagiário/Projetista</t>
+          <t>Eng. Sênior</t>
         </is>
       </c>
       <c r="C103" s="7" t="inlineStr">
         <is>
-          <t>Sinalização</t>
+          <t>Pavimento</t>
         </is>
       </c>
       <c r="D103" s="8" t="n">
@@ -2492,17 +2526,17 @@
     <row r="104">
       <c r="A104" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="B104" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Eng. Pleno</t>
         </is>
       </c>
       <c r="C104" s="7" t="inlineStr">
         <is>
-          <t>Sinalização</t>
+          <t>Pavimento</t>
         </is>
       </c>
       <c r="D104" s="8" t="n">
@@ -2516,17 +2550,17 @@
     <row r="105">
       <c r="A105" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="B105" s="7" t="inlineStr">
         <is>
-          <t>Eng. Pleno</t>
+          <t>Eng. Júnior</t>
         </is>
       </c>
       <c r="C105" s="7" t="inlineStr">
         <is>
-          <t>Sinalização</t>
+          <t>Pavimento</t>
         </is>
       </c>
       <c r="D105" s="8" t="n">
@@ -2540,17 +2574,17 @@
     <row r="106">
       <c r="A106" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="B106" s="7" t="inlineStr">
         <is>
-          <t>Eng. Júnior</t>
+          <t>Coordenador</t>
         </is>
       </c>
       <c r="C106" s="7" t="inlineStr">
         <is>
-          <t>Sinalização</t>
+          <t>Pavimento</t>
         </is>
       </c>
       <c r="D106" s="8" t="n">
@@ -2562,74 +2596,57 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="7" t="inlineStr">
-        <is>
-          <t>Coordenador</t>
-        </is>
-      </c>
-      <c r="B107" s="7" t="inlineStr">
-        <is>
-          <t>Coordenador</t>
-        </is>
-      </c>
-      <c r="C107" s="7" t="inlineStr">
+      <c r="A107" s="6" t="inlineStr">
+        <is>
+          <t>Proejto ANTT Pav.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="7" t="inlineStr">
+        <is>
+          <t>resre</t>
+        </is>
+      </c>
+      <c r="B108" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C108" s="7" t="inlineStr">
+        <is>
+          <t>Proejto ANTT Pav.</t>
+        </is>
+      </c>
+      <c r="D108" s="8" t="n">
+        <v>320</v>
+      </c>
+      <c r="E108" s="9">
+        <f>IFERROR(VLOOKUP(B108,TabelaPrecos,2,FALSE)*D108,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="6" t="inlineStr">
         <is>
           <t>Sinalização</t>
         </is>
-      </c>
-      <c r="D107" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="9">
-        <f>IFERROR(VLOOKUP(B107,TabelaPrecos,2,FALSE)*D107,"-")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="6" t="inlineStr">
-        <is>
-          <t>Terraplenagem</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="B109" s="7" t="inlineStr">
-        <is>
-          <t>Estagiário/Projetista</t>
-        </is>
-      </c>
-      <c r="C109" s="7" t="inlineStr">
-        <is>
-          <t>Terraplenagem</t>
-        </is>
-      </c>
-      <c r="D109" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="9">
-        <f>IFERROR(VLOOKUP(B109,TabelaPrecos,2,FALSE)*D109,"-")</f>
-        <v/>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="B110" s="7" t="inlineStr">
         <is>
-          <t>Eng. Sênior</t>
+          <t>Estagiário/Projetista</t>
         </is>
       </c>
       <c r="C110" s="7" t="inlineStr">
         <is>
-          <t>Terraplenagem</t>
+          <t>Sinalização</t>
         </is>
       </c>
       <c r="D110" s="8" t="n">
@@ -2653,7 +2670,7 @@
       </c>
       <c r="C111" s="7" t="inlineStr">
         <is>
-          <t>Terraplenagem</t>
+          <t>Sinalização</t>
         </is>
       </c>
       <c r="D111" s="8" t="n">
@@ -2677,7 +2694,7 @@
       </c>
       <c r="C112" s="7" t="inlineStr">
         <is>
-          <t>Terraplenagem</t>
+          <t>Sinalização</t>
         </is>
       </c>
       <c r="D112" s="8" t="n">
@@ -2701,7 +2718,7 @@
       </c>
       <c r="C113" s="7" t="inlineStr">
         <is>
-          <t>Terraplenagem</t>
+          <t>Sinalização</t>
         </is>
       </c>
       <c r="D113" s="8" t="n">
@@ -2713,247 +2730,309 @@
       </c>
     </row>
     <row r="114">
-      <c r="D114" s="10" t="inlineStr">
+      <c r="A114" s="6" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="B115" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C115" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="D115" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="9">
+        <f>IFERROR(VLOOKUP(B115,TabelaPrecos,2,FALSE)*D115,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="B116" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="C116" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="D116" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="9">
+        <f>IFERROR(VLOOKUP(B116,TabelaPrecos,2,FALSE)*D116,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="B117" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C117" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="D117" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="9">
+        <f>IFERROR(VLOOKUP(B117,TabelaPrecos,2,FALSE)*D117,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="B118" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C118" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="D118" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="9">
+        <f>IFERROR(VLOOKUP(B118,TabelaPrecos,2,FALSE)*D118,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B119" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C119" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="D119" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" s="9">
+        <f>IFERROR(VLOOKUP(B119,TabelaPrecos,2,FALSE)*D119,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="6" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="B121" s="7" t="inlineStr">
+        <is>
+          <t>Estagiário/Projetista</t>
+        </is>
+      </c>
+      <c r="C121" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="D121" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" s="9">
+        <f>IFERROR(VLOOKUP(B121,TabelaPrecos,2,FALSE)*D121,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="B122" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Sênior</t>
+        </is>
+      </c>
+      <c r="C122" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="D122" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" s="9">
+        <f>IFERROR(VLOOKUP(B122,TabelaPrecos,2,FALSE)*D122,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="B123" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Pleno</t>
+        </is>
+      </c>
+      <c r="C123" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="D123" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" s="9">
+        <f>IFERROR(VLOOKUP(B123,TabelaPrecos,2,FALSE)*D123,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="B124" s="7" t="inlineStr">
+        <is>
+          <t>Eng. Júnior</t>
+        </is>
+      </c>
+      <c r="C124" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="D124" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" s="9">
+        <f>IFERROR(VLOOKUP(B124,TabelaPrecos,2,FALSE)*D124,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="B125" s="7" t="inlineStr">
+        <is>
+          <t>Coordenador</t>
+        </is>
+      </c>
+      <c r="C125" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="D125" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" s="9">
+        <f>IFERROR(VLOOKUP(B125,TabelaPrecos,2,FALSE)*D125,"-")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126">
+      <c r="D126" s="10" t="inlineStr">
         <is>
           <t>Total Geral</t>
         </is>
       </c>
-      <c r="E114" s="11">
-        <f>SUM(E12:E113)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="115"/>
-    <row r="116"/>
-    <row r="117">
-      <c r="B117" s="1" t="inlineStr">
+      <c r="E126" s="11">
+        <f>SUM(E12:E125)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129">
+      <c r="B129" s="1" t="inlineStr">
         <is>
           <t>Resumo Financeiro por Disciplina</t>
         </is>
       </c>
     </row>
-    <row r="118">
-      <c r="B118" s="5" t="inlineStr">
+    <row r="130">
+      <c r="B130" s="5" t="inlineStr">
         <is>
           <t>Disciplina</t>
         </is>
       </c>
-      <c r="C118" s="5" t="inlineStr">
+      <c r="C130" s="5" t="inlineStr">
         <is>
           <t>Total HH (R$)</t>
         </is>
       </c>
-      <c r="D118" s="5" t="inlineStr">
+      <c r="D130" s="5" t="inlineStr">
         <is>
           <t>Total por Desenho (R$)</t>
         </is>
       </c>
-      <c r="E118" s="5" t="inlineStr">
+      <c r="E130" s="5" t="inlineStr">
         <is>
           <t>Subtotal (R$)</t>
         </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="B119" s="7" t="inlineStr">
-        <is>
-          <t>Acompanhamento de Sondagens</t>
-        </is>
-      </c>
-      <c r="C119" s="9">
-        <f>SUMIF(C$12:C$113, B119, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D119" s="4" t="n"/>
-      <c r="E119" s="9">
-        <f>C119-D119</f>
-        <v/>
-      </c>
-    </row>
-    <row r="120">
-      <c r="B120" s="7" t="inlineStr">
-        <is>
-          <t>Coordenação</t>
-        </is>
-      </c>
-      <c r="C120" s="9">
-        <f>SUMIF(C$12:C$113, B120, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D120" s="4" t="n"/>
-      <c r="E120" s="9">
-        <f>C120-D120</f>
-        <v/>
-      </c>
-    </row>
-    <row r="121">
-      <c r="B121" s="7" t="inlineStr">
-        <is>
-          <t>Estruturas</t>
-        </is>
-      </c>
-      <c r="C121" s="9">
-        <f>SUMIF(C$12:C$113, B121, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D121" s="4" t="n"/>
-      <c r="E121" s="9">
-        <f>C121-D121</f>
-        <v/>
-      </c>
-    </row>
-    <row r="122">
-      <c r="B122" s="7" t="inlineStr">
-        <is>
-          <t>Estudo de Alternativa</t>
-        </is>
-      </c>
-      <c r="C122" s="9">
-        <f>SUMIF(C$12:C$113, B122, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D122" s="4" t="n"/>
-      <c r="E122" s="9">
-        <f>C122-D122</f>
-        <v/>
-      </c>
-    </row>
-    <row r="123">
-      <c r="B123" s="7" t="inlineStr">
-        <is>
-          <t>Estudos Geológicos-Geotécnicos</t>
-        </is>
-      </c>
-      <c r="C123" s="9">
-        <f>SUMIF(C$12:C$113, B123, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D123" s="4" t="n"/>
-      <c r="E123" s="9">
-        <f>C123-D123</f>
-        <v/>
-      </c>
-    </row>
-    <row r="124">
-      <c r="B124" s="7" t="inlineStr">
-        <is>
-          <t>Geologia</t>
-        </is>
-      </c>
-      <c r="C124" s="9">
-        <f>SUMIF(C$12:C$113, B124, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D124" s="4" t="n"/>
-      <c r="E124" s="9">
-        <f>C124-D124</f>
-        <v/>
-      </c>
-    </row>
-    <row r="125">
-      <c r="B125" s="7" t="inlineStr">
-        <is>
-          <t>Geometria</t>
-        </is>
-      </c>
-      <c r="C125" s="9">
-        <f>SUMIF(C$12:C$113, B125, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D125" s="4" t="n"/>
-      <c r="E125" s="9">
-        <f>C125-D125</f>
-        <v/>
-      </c>
-    </row>
-    <row r="126">
-      <c r="B126" s="7" t="inlineStr">
-        <is>
-          <t>Geotecnia</t>
-        </is>
-      </c>
-      <c r="C126" s="9">
-        <f>SUMIF(C$12:C$113, B126, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D126" s="4" t="n"/>
-      <c r="E126" s="9">
-        <f>C126-D126</f>
-        <v/>
-      </c>
-    </row>
-    <row r="127">
-      <c r="B127" s="7" t="inlineStr">
-        <is>
-          <t>Pavimento</t>
-        </is>
-      </c>
-      <c r="C127" s="9">
-        <f>SUMIF(C$12:C$113, B127, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D127" s="4" t="n"/>
-      <c r="E127" s="9">
-        <f>C127-D127</f>
-        <v/>
-      </c>
-    </row>
-    <row r="128">
-      <c r="B128" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Desapropriação</t>
-        </is>
-      </c>
-      <c r="C128" s="9">
-        <f>SUMIF(C$12:C$113, B128, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D128" s="4" t="n"/>
-      <c r="E128" s="9">
-        <f>C128-D128</f>
-        <v/>
-      </c>
-    </row>
-    <row r="129">
-      <c r="B129" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Interferência</t>
-        </is>
-      </c>
-      <c r="C129" s="9">
-        <f>SUMIF(C$12:C$113, B129, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D129" s="4" t="n"/>
-      <c r="E129" s="9">
-        <f>C129-D129</f>
-        <v/>
-      </c>
-    </row>
-    <row r="130">
-      <c r="B130" s="7" t="inlineStr">
-        <is>
-          <t>Projeto de Obras Complementares</t>
-        </is>
-      </c>
-      <c r="C130" s="9">
-        <f>SUMIF(C$12:C$113, B130, E$12:E$113)</f>
-        <v/>
-      </c>
-      <c r="D130" s="4" t="n"/>
-      <c r="E130" s="9">
-        <f>C130-D130</f>
-        <v/>
       </c>
     </row>
     <row r="131">
       <c r="B131" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Paisagismo</t>
+          <t>Consolidação e Identificação de Interferências</t>
         </is>
       </c>
       <c r="C131" s="9">
-        <f>SUMIF(C$12:C$113, B131, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B131, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D131" s="4" t="n"/>
@@ -2965,11 +3044,11 @@
     <row r="132">
       <c r="B132" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Parada de Ônibus</t>
+          <t>Coordenação</t>
         </is>
       </c>
       <c r="C132" s="9">
-        <f>SUMIF(C$12:C$113, B132, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B132, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D132" s="4" t="n"/>
@@ -2981,11 +3060,11 @@
     <row r="133">
       <c r="B133" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Passarelas e de Pedestres</t>
+          <t>Desapropriação</t>
         </is>
       </c>
       <c r="C133" s="9">
-        <f>SUMIF(C$12:C$113, B133, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B133, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D133" s="4" t="n"/>
@@ -2997,11 +3076,11 @@
     <row r="134">
       <c r="B134" s="7" t="inlineStr">
         <is>
-          <t>Projeto de Topografia</t>
+          <t>Drenagem</t>
         </is>
       </c>
       <c r="C134" s="9">
-        <f>SUMIF(C$12:C$113, B134, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B134, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D134" s="4" t="n"/>
@@ -3013,11 +3092,11 @@
     <row r="135">
       <c r="B135" s="7" t="inlineStr">
         <is>
-          <t>Sinalização</t>
+          <t>Estruturas</t>
         </is>
       </c>
       <c r="C135" s="9">
-        <f>SUMIF(C$12:C$113, B135, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B135, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D135" s="4" t="n"/>
@@ -3029,11 +3108,11 @@
     <row r="136">
       <c r="B136" s="7" t="inlineStr">
         <is>
-          <t>Terraplenagem</t>
+          <t>Estudo de Alternativa</t>
         </is>
       </c>
       <c r="C136" s="9">
-        <f>SUMIF(C$12:C$113, B136, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B136, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D136" s="4" t="n"/>
@@ -3045,11 +3124,11 @@
     <row r="137">
       <c r="B137" s="7" t="inlineStr">
         <is>
-          <t>Drenagem</t>
+          <t>Estudos Geológicos-Geotécnicos</t>
         </is>
       </c>
       <c r="C137" s="9">
-        <f>SUMIF(C$12:C$113, B137, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B137, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D137" s="4" t="n"/>
@@ -3065,7 +3144,7 @@
         </is>
       </c>
       <c r="C138" s="9">
-        <f>SUMIF(C$12:C$113, B138, E$12:E$113)</f>
+        <f>SUMIF(C$12:C$125, B138, E$12:E$125)</f>
         <v/>
       </c>
       <c r="D138" s="4" t="n"/>
@@ -3075,38 +3154,247 @@
       </c>
     </row>
     <row r="139">
-      <c r="D139" s="12" t="inlineStr">
+      <c r="B139" s="7" t="inlineStr">
+        <is>
+          <t>Geologia</t>
+        </is>
+      </c>
+      <c r="C139" s="9">
+        <f>SUMIF(C$12:C$125, B139, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D139" s="4" t="n"/>
+      <c r="E139" s="9">
+        <f>C139-D139</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" s="7" t="inlineStr">
+        <is>
+          <t>Geometria</t>
+        </is>
+      </c>
+      <c r="C140" s="9">
+        <f>SUMIF(C$12:C$125, B140, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D140" s="4" t="n"/>
+      <c r="E140" s="9">
+        <f>C140-D140</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" s="7" t="inlineStr">
+        <is>
+          <t>Geotecnia</t>
+        </is>
+      </c>
+      <c r="C141" s="9">
+        <f>SUMIF(C$12:C$125, B141, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D141" s="4" t="n"/>
+      <c r="E141" s="9">
+        <f>C141-D141</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" s="7" t="inlineStr">
+        <is>
+          <t>Interferência</t>
+        </is>
+      </c>
+      <c r="C142" s="9">
+        <f>SUMIF(C$12:C$125, B142, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D142" s="4" t="n"/>
+      <c r="E142" s="9">
+        <f>C142-D142</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" s="7" t="inlineStr">
+        <is>
+          <t>Obras Complementares</t>
+        </is>
+      </c>
+      <c r="C143" s="9">
+        <f>SUMIF(C$12:C$125, B143, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D143" s="4" t="n"/>
+      <c r="E143" s="9">
+        <f>C143-D143</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" s="7" t="inlineStr">
+        <is>
+          <t>Paisagismo</t>
+        </is>
+      </c>
+      <c r="C144" s="9">
+        <f>SUMIF(C$12:C$125, B144, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D144" s="4" t="n"/>
+      <c r="E144" s="9">
+        <f>C144-D144</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" s="7" t="inlineStr">
+        <is>
+          <t>Parada de Ônibus</t>
+        </is>
+      </c>
+      <c r="C145" s="9">
+        <f>SUMIF(C$12:C$125, B145, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D145" s="4" t="n"/>
+      <c r="E145" s="9">
+        <f>C145-D145</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" s="7" t="inlineStr">
+        <is>
+          <t>Passarelas e de Pedestres</t>
+        </is>
+      </c>
+      <c r="C146" s="9">
+        <f>SUMIF(C$12:C$125, B146, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D146" s="4" t="n"/>
+      <c r="E146" s="9">
+        <f>C146-D146</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" s="7" t="inlineStr">
+        <is>
+          <t>Pavimento</t>
+        </is>
+      </c>
+      <c r="C147" s="9">
+        <f>SUMIF(C$12:C$125, B147, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D147" s="4" t="n"/>
+      <c r="E147" s="9">
+        <f>C147-D147</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" s="7" t="inlineStr">
+        <is>
+          <t>Sinalização</t>
+        </is>
+      </c>
+      <c r="C148" s="9">
+        <f>SUMIF(C$12:C$125, B148, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D148" s="4" t="n"/>
+      <c r="E148" s="9">
+        <f>C148-D148</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" s="7" t="inlineStr">
+        <is>
+          <t>Terraplenagem</t>
+        </is>
+      </c>
+      <c r="C149" s="9">
+        <f>SUMIF(C$12:C$125, B149, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D149" s="4" t="n"/>
+      <c r="E149" s="9">
+        <f>C149-D149</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" s="7" t="inlineStr">
+        <is>
+          <t>Topografia</t>
+        </is>
+      </c>
+      <c r="C150" s="9">
+        <f>SUMIF(C$12:C$125, B150, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D150" s="4" t="n"/>
+      <c r="E150" s="9">
+        <f>C150-D150</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" s="7" t="inlineStr">
+        <is>
+          <t>Proejto ANTT Pav.</t>
+        </is>
+      </c>
+      <c r="C151" s="9">
+        <f>SUMIF(C$12:C$125, B151, E$12:E$125)</f>
+        <v/>
+      </c>
+      <c r="D151" s="4" t="n"/>
+      <c r="E151" s="9">
+        <f>C151-D151</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152">
+      <c r="D152" s="12" t="inlineStr">
         <is>
           <t>Total Final</t>
         </is>
       </c>
-      <c r="E139" s="13">
-        <f>SUM(E119:E138)</f>
+      <c r="E152" s="13">
+        <f>SUM(E131:E151)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
     <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A78:E78"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A41:E41"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A108:E108"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="A114:E114"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A65:E65"/>
     <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A120:E120"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A62:E62"/>
-    <mergeCell ref="A96:E96"/>
-    <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A76:E76"/>
+    <mergeCell ref="A71:E71"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A97:E97"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A109:E109"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>